<commit_message>
Data update, added update dates
</commit_message>
<xml_diff>
--- a/public/ECF-buildings-dashboard-data.xlsx
+++ b/public/ECF-buildings-dashboard-data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5270" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5270" uniqueCount="623">
   <si>
     <t>geo</t>
   </si>
@@ -1879,9 +1879,6 @@
   </si>
   <si>
     <t>RRF</t>
-  </si>
-  <si>
-    <t>submitted / not yet assessed</t>
   </si>
   <si>
     <t>submitted / assessed</t>
@@ -40810,19 +40807,19 @@
         <v>620</v>
       </c>
       <c r="D2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I2" t="s">
         <v>587</v>
@@ -40839,19 +40836,19 @@
         <v>620</v>
       </c>
       <c r="D3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I3" t="s">
         <v>588</v>
@@ -40865,22 +40862,22 @@
         <v>441</v>
       </c>
       <c r="C4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I4" t="s">
         <v>589</v>
@@ -40894,22 +40891,22 @@
         <v>442</v>
       </c>
       <c r="C5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I5" t="s">
         <v>590</v>
@@ -40923,22 +40920,22 @@
         <v>432</v>
       </c>
       <c r="C6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I6" t="s">
         <v>591</v>
@@ -40952,22 +40949,22 @@
         <v>443</v>
       </c>
       <c r="C7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I7" t="s">
         <v>592</v>
@@ -40984,19 +40981,19 @@
         <v>620</v>
       </c>
       <c r="D8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I8" t="s">
         <v>593</v>
@@ -41010,22 +41007,22 @@
         <v>445</v>
       </c>
       <c r="C9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I9" t="s">
         <v>594</v>
@@ -41039,22 +41036,22 @@
         <v>448</v>
       </c>
       <c r="C10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I10" t="s">
         <v>595</v>
@@ -41071,19 +41068,19 @@
         <v>620</v>
       </c>
       <c r="D11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I11" t="s">
         <v>596</v>
@@ -41097,22 +41094,22 @@
         <v>433</v>
       </c>
       <c r="C12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I12" t="s">
         <v>597</v>
@@ -41129,19 +41126,19 @@
         <v>620</v>
       </c>
       <c r="D13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I13" t="s">
         <v>598</v>
@@ -41155,22 +41152,22 @@
         <v>440</v>
       </c>
       <c r="C14" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I14" t="s">
         <v>599</v>
@@ -41187,19 +41184,19 @@
         <v>620</v>
       </c>
       <c r="D15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I15" t="s">
         <v>600</v>
@@ -41216,19 +41213,19 @@
         <v>620</v>
       </c>
       <c r="D16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I16" t="s">
         <v>601</v>
@@ -41242,22 +41239,22 @@
         <v>453</v>
       </c>
       <c r="C17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I17" t="s">
         <v>602</v>
@@ -41271,22 +41268,22 @@
         <v>450</v>
       </c>
       <c r="C18" t="s">
+        <v>620</v>
+      </c>
+      <c r="D18" t="s">
         <v>622</v>
       </c>
-      <c r="D18" t="s">
-        <v>623</v>
-      </c>
       <c r="E18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I18" t="s">
         <v>603</v>
@@ -41300,22 +41297,22 @@
         <v>454</v>
       </c>
       <c r="C19" t="s">
+        <v>620</v>
+      </c>
+      <c r="D19" t="s">
         <v>622</v>
       </c>
-      <c r="D19" t="s">
-        <v>623</v>
-      </c>
       <c r="E19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I19" t="s">
         <v>604</v>
@@ -41329,22 +41326,22 @@
         <v>455</v>
       </c>
       <c r="C20" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D20" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E20" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F20" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G20" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H20" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I20" t="s">
         <v>605</v>
@@ -41358,22 +41355,22 @@
         <v>431</v>
       </c>
       <c r="C21" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I21" t="s">
         <v>606</v>
@@ -41387,22 +41384,22 @@
         <v>435</v>
       </c>
       <c r="C22" t="s">
+        <v>621</v>
+      </c>
+      <c r="D22" t="s">
         <v>622</v>
       </c>
-      <c r="D22" t="s">
-        <v>623</v>
-      </c>
       <c r="E22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I22" t="s">
         <v>607</v>
@@ -41419,19 +41416,19 @@
         <v>620</v>
       </c>
       <c r="D23" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E23" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F23" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G23" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H23" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I23" t="s">
         <v>608</v>
@@ -41448,19 +41445,19 @@
         <v>620</v>
       </c>
       <c r="D24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I24" t="s">
         <v>609</v>
@@ -41474,22 +41471,22 @@
         <v>457</v>
       </c>
       <c r="C25" t="s">
+        <v>620</v>
+      </c>
+      <c r="D25" t="s">
         <v>622</v>
       </c>
-      <c r="D25" t="s">
-        <v>623</v>
-      </c>
       <c r="E25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I25" t="s">
         <v>610</v>
@@ -41506,19 +41503,19 @@
         <v>620</v>
       </c>
       <c r="D26" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E26" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F26" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G26" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H26" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I26" t="s">
         <v>611</v>
@@ -41532,22 +41529,22 @@
         <v>447</v>
       </c>
       <c r="C27" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D27" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E27" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F27" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G27" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H27" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I27" t="s">
         <v>612</v>
@@ -41561,22 +41558,22 @@
         <v>456</v>
       </c>
       <c r="C28" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I28" t="s">
         <v>613</v>

</xml_diff>